<commit_message>
add parameter to setting
</commit_message>
<xml_diff>
--- a/database/industries/felezat/fameli/income/quarterly/rial.xlsx
+++ b/database/industries/felezat/fameli/income/quarterly/rial.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\EBRAHIMI\Desktop\Trade\database\industries\felezat\fameli\income\quarterly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\felezat\fameli\income\quarterly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEA9173-EBE0-4730-9BA8-921108025288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -154,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -614,10 +613,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1395,7 +1396,8 @@
         <v>400000000</v>
       </c>
       <c r="M26" s="11">
-        <v>400000000</v>
+        <f>L26*1.5</f>
+        <v>600000000</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>